<commit_message>
Fixed bug in array expansion
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="Named_reference">Referencing!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -756,27 +756,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1">
         <f>C4</f>
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2">
         <f>Named_reference</f>
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>10</v>
       </c>
@@ -789,30 +789,124 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6">
       <c r="A5">
         <f>1+1+1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:6">
       <c r="B8">
         <f ca="1">INDIRECT("naMed_reFerence")</f>
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:6">
       <c r="B9">
         <f ca="1">SUM(INDIRECT("firsttable[#Totals]"))</f>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16">
+        <v>1.4535833325868115</v>
+      </c>
+      <c r="D16">
+        <v>1.4535833325868115</v>
+      </c>
+      <c r="E16">
+        <v>1.5117266658902839</v>
+      </c>
+      <c r="F16">
+        <v>1.5407983325420203</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17">
+        <v>9.0545454545454547</v>
+      </c>
+      <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17">
+        <v>18</v>
+      </c>
+      <c r="F17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18">
+        <v>0.36811506356713858</v>
+      </c>
+      <c r="D18">
+        <v>0.36811506356713858</v>
+      </c>
+      <c r="E18">
+        <v>0.40588480110308967</v>
+      </c>
+      <c r="F18">
+        <v>0.42190146532760275</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="D19">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="E19">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="F19">
+        <v>0.65100000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <f t="array" ref="D22:D25">INDEX(C16:F19,,MATCH(C22,C15:F15,0))</f>
+        <v>1.5407983325420203</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="D23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="D24">
+        <v>0.42190146532760275</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="D25">
+        <v>0.65100000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed another bug in array formulae expansion
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>Hello</t>
   </si>
@@ -84,13 +84,143 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>Technology efficiencies -- hot water -- annual mean</t>
+  </si>
+  <si>
+    <t>% of input energy</t>
+  </si>
+  <si>
+    <t>Electricity (delivered to end user)</t>
+  </si>
+  <si>
+    <t>Electricity (supplied to grid)</t>
+  </si>
+  <si>
+    <t>Solid hydrocarbons</t>
+  </si>
+  <si>
+    <t>Liquid hydrocarbons</t>
+  </si>
+  <si>
+    <t>Gaseous hydrocarbons</t>
+  </si>
+  <si>
+    <t>Heat transport</t>
+  </si>
+  <si>
+    <t>Environmental heat</t>
+  </si>
+  <si>
+    <t>Heating &amp; cooling</t>
+  </si>
+  <si>
+    <t>Conversion losses</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>V.01</t>
+  </si>
+  <si>
+    <t>V.02</t>
+  </si>
+  <si>
+    <t>V.03</t>
+  </si>
+  <si>
+    <t>V.04</t>
+  </si>
+  <si>
+    <t>V.05</t>
+  </si>
+  <si>
+    <t>V.07</t>
+  </si>
+  <si>
+    <t>R.07</t>
+  </si>
+  <si>
+    <t>H.01</t>
+  </si>
+  <si>
+    <t>X.01</t>
+  </si>
+  <si>
+    <t>Gas boiler (old)</t>
+  </si>
+  <si>
+    <t>Gas boiler (new)</t>
+  </si>
+  <si>
+    <t>Resistive heating</t>
+  </si>
+  <si>
+    <t>Oil-fired boiler</t>
+  </si>
+  <si>
+    <t>Solid-fuel boiler</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>Stirling engine micro-CHP</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>Fuel-cell micro-CHP</t>
+  </si>
+  <si>
+    <t>Air-source heat pump</t>
+  </si>
+  <si>
+    <t>Ground-source heat pump</t>
+  </si>
+  <si>
+    <t>Geothermal electricity</t>
+  </si>
+  <si>
+    <t>Community scale gas CHP with local district heating</t>
+  </si>
+  <si>
+    <t>Community scale solid-fuel CHP with local district heating</t>
+  </si>
+  <si>
+    <t>Long distance district heating from large power stations</t>
+  </si>
+  <si>
+    <t>[6]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,29 +262,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="18">
+    <cellStyle name="Comma" xfId="17" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -756,10 +896,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -843,7 +983,7 @@
         <v>1.5407983325420203</v>
       </c>
     </row>
-    <row r="17" spans="3:6">
+    <row r="17" spans="3:15">
       <c r="C17">
         <v>9.0545454545454547</v>
       </c>
@@ -857,7 +997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:6">
+    <row r="18" spans="3:15">
       <c r="C18">
         <v>0.36811506356713858</v>
       </c>
@@ -871,7 +1011,7 @@
         <v>0.42190146532760275</v>
       </c>
     </row>
-    <row r="19" spans="3:6">
+    <row r="19" spans="3:15">
       <c r="C19">
         <v>0.65100000000000002</v>
       </c>
@@ -885,7 +1025,7 @@
         <v>0.65100000000000002</v>
       </c>
     </row>
-    <row r="22" spans="3:6">
+    <row r="22" spans="3:15">
       <c r="C22">
         <v>4</v>
       </c>
@@ -894,19 +1034,499 @@
         <v>1.5407983325420203</v>
       </c>
     </row>
-    <row r="23" spans="3:6">
+    <row r="23" spans="3:15">
       <c r="D23">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="3:6">
+    <row r="24" spans="3:15">
       <c r="D24">
         <v>0.42190146532760275</v>
       </c>
     </row>
-    <row r="25" spans="3:6">
+    <row r="25" spans="3:15">
       <c r="D25">
         <v>0.65100000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15">
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="O31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15">
+      <c r="F33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" t="s">
+        <v>28</v>
+      </c>
+      <c r="N33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15">
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" t="s">
+        <v>36</v>
+      </c>
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M34" t="s">
+        <v>41</v>
+      </c>
+      <c r="N34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J35">
+        <v>-1</v>
+      </c>
+      <c r="M35">
+        <v>0.76</v>
+      </c>
+      <c r="N35">
+        <v>0.24</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15">
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="J36">
+        <v>-1</v>
+      </c>
+      <c r="M36">
+        <v>0.91</v>
+      </c>
+      <c r="N36">
+        <v>0.09</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:15">
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37">
+        <v>-1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15">
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+      <c r="I38">
+        <v>-1</v>
+      </c>
+      <c r="M38">
+        <v>0.97</v>
+      </c>
+      <c r="N38">
+        <v>0.03</v>
+      </c>
+      <c r="O38">
+        <v>-2.7755575615628914E-17</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15">
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" t="s">
+        <v>48</v>
+      </c>
+      <c r="H39">
+        <v>-1</v>
+      </c>
+      <c r="M39">
+        <v>0.87</v>
+      </c>
+      <c r="N39">
+        <v>0.13</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:15">
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="J40">
+        <v>-1</v>
+      </c>
+      <c r="M40">
+        <v>0.63</v>
+      </c>
+      <c r="N40">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:15">
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41">
+        <v>0.45</v>
+      </c>
+      <c r="J41">
+        <v>-1</v>
+      </c>
+      <c r="M41">
+        <v>0.45</v>
+      </c>
+      <c r="N41">
+        <v>0.1</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15">
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42">
+        <v>-1</v>
+      </c>
+      <c r="L42">
+        <v>-1</v>
+      </c>
+      <c r="M42">
+        <v>2</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15">
+      <c r="C43">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43">
+        <v>-1</v>
+      </c>
+      <c r="L43">
+        <v>-2</v>
+      </c>
+      <c r="M43">
+        <v>3</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:15">
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>54</v>
+      </c>
+      <c r="L44">
+        <v>-1</v>
+      </c>
+      <c r="M44">
+        <v>0.85</v>
+      </c>
+      <c r="N44">
+        <v>0.15</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:15">
+      <c r="C45">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>55</v>
+      </c>
+      <c r="G45">
+        <v>0.38</v>
+      </c>
+      <c r="J45">
+        <v>-1</v>
+      </c>
+      <c r="M45">
+        <v>0.38</v>
+      </c>
+      <c r="N45">
+        <v>0.24</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="3:15">
+      <c r="C46">
+        <v>12</v>
+      </c>
+      <c r="D46" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46">
+        <v>0.17</v>
+      </c>
+      <c r="H46">
+        <v>-1</v>
+      </c>
+      <c r="M46">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N46">
+        <v>0.26</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="3:15">
+      <c r="C47">
+        <v>13</v>
+      </c>
+      <c r="D47" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" t="s">
+        <v>58</v>
+      </c>
+      <c r="K47">
+        <v>-1</v>
+      </c>
+      <c r="M47">
+        <v>0.9</v>
+      </c>
+      <c r="N47">
+        <v>0.1</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:8">
+      <c r="D50" t="s">
+        <v>43</v>
+      </c>
+      <c r="G50">
+        <v>137.26515207025273</v>
+      </c>
+    </row>
+    <row r="51" spans="4:8">
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+      <c r="G51">
+        <v>30.731004194832696</v>
+      </c>
+    </row>
+    <row r="52" spans="4:8">
+      <c r="D52" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52">
+        <v>20.487336129888465</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8">
+      <c r="D53" t="s">
+        <v>46</v>
+      </c>
+      <c r="G53">
+        <v>8.1949344519553868</v>
+      </c>
+    </row>
+    <row r="54" spans="4:8">
+      <c r="D54" t="s">
+        <v>47</v>
+      </c>
+      <c r="G54">
+        <v>8.1949344519553868</v>
+      </c>
+    </row>
+    <row r="55" spans="4:8">
+      <c r="D55" t="s">
+        <v>49</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:8">
+      <c r="D56" t="s">
+        <v>51</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="4:8">
+      <c r="D57" t="s">
+        <v>52</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:8">
+      <c r="D58" t="s">
+        <v>53</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="4:8">
+      <c r="D59" t="s">
+        <v>54</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:8">
+      <c r="D60" t="s">
+        <v>55</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="4:8">
+      <c r="D61" t="s">
+        <v>56</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="4:8">
+      <c r="D62" t="s">
+        <v>57</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="4:8">
+      <c r="D64" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="4">
+        <f t="array" ref="H64">SUM(G$50:G$62/$M$35:$M$47*($D64=$F$34:$N$34)*($F$35:$N$47))</f>
+        <v>204.87336129888465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a bodge to deal with INDIRECTS that exist within array formulae. This will, no doubt, haunt me.
</commit_message>
<xml_diff>
--- a/spec/test_data/ExampleSpreadsheet.xlsx
+++ b/spec/test_data/ExampleSpreadsheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Hello</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>[6]</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Gamma</t>
   </si>
 </sst>
 </file>
@@ -896,10 +905,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1527,6 +1536,43 @@
       <c r="H64" s="4">
         <f t="array" ref="H64">SUM(G$50:G$62/$M$35:$M$47*($D64=$F$34:$N$34)*($F$35:$N$47))</f>
         <v>204.87336129888465</v>
+      </c>
+    </row>
+    <row r="68" spans="5:7">
+      <c r="E68" t="s">
+        <v>59</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="5:7">
+      <c r="E69" t="s">
+        <v>60</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="5:7">
+      <c r="E70" t="s">
+        <v>61</v>
+      </c>
+      <c r="F70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="5:7">
+      <c r="E72" t="s">
+        <v>60</v>
+      </c>
+      <c r="F72">
+        <f t="array" ref="F72">SUM((E72=$E$68:$E$70)*$F$68:$F$70)</f>
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <f t="array" aca="1" ref="G72" ca="1">SUM((E72=$E$68:$E$70)*INDIRECT("$F$68:$F$70"))</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>